<commit_message>
addl images and and colorscheme
</commit_message>
<xml_diff>
--- a/geometry/bob/bob_color_scheme.xlsx
+++ b/geometry/bob/bob_color_scheme.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chovey/autotwin/ssm/geometry/bob/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FB8CC8-AC5C-0D42-B429-CBE8F86FE10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A25032-215F-D442-BCB4-403DA70E5B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{5ECDCC65-078E-8E42-91F9-0C729C03B2F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA5A6BD-463E-074A-86C7-158E5D17EE3A}">
   <dimension ref="C25:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,15 +667,15 @@
         <v>0.70199999999999996</v>
       </c>
       <c r="F26" s="5">
-        <f>C26*255</f>
+        <f t="shared" ref="F26:F35" si="0">C26*255</f>
         <v>245.05499999999998</v>
       </c>
       <c r="G26" s="5">
-        <f>D26*255</f>
+        <f t="shared" ref="G26:G35" si="1">D26*255</f>
         <v>222.10499999999999</v>
       </c>
       <c r="H26" s="6">
-        <f>E26*255</f>
+        <f t="shared" ref="H26:H35" si="2">E26*255</f>
         <v>179.01</v>
       </c>
       <c r="I26" s="2">
@@ -696,15 +696,15 @@
         <v>0</v>
       </c>
       <c r="F27" s="5">
-        <f>C27*255</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="G27" s="5">
-        <f>D27*255</f>
+        <f t="shared" si="1"/>
         <v>164.98500000000001</v>
       </c>
       <c r="H27" s="6">
-        <f>E27*255</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I27" s="3">
@@ -726,19 +726,19 @@
         <v>0</v>
       </c>
       <c r="F28" s="5">
-        <f>C28*255</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="G28" s="5">
-        <f>D28*255</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H28" s="6">
-        <f>E28*255</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" ref="I28:I37" si="0">I27+1</f>
+        <f t="shared" ref="I28:I35" si="3">I27+1</f>
         <v>3</v>
       </c>
       <c r="J28" s="1" t="s">
@@ -756,19 +756,19 @@
         <v>0.184</v>
       </c>
       <c r="F29" s="5">
-        <f>C29*255</f>
+        <f t="shared" si="0"/>
         <v>84.915000000000006</v>
       </c>
       <c r="G29" s="5">
-        <f>D29*255</f>
+        <f t="shared" si="1"/>
         <v>107.1</v>
       </c>
       <c r="H29" s="6">
-        <f>E29*255</f>
+        <f t="shared" si="2"/>
         <v>46.92</v>
       </c>
       <c r="I29" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J29" s="1" t="s">
@@ -786,19 +786,19 @@
         <v>0</v>
       </c>
       <c r="F30" s="1">
-        <f>C30*255</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="G30" s="5">
-        <f>D30*255</f>
+        <f t="shared" si="1"/>
         <v>214.965</v>
       </c>
       <c r="H30" s="1">
-        <f>E30*255</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I30" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J30" s="1" t="s">
@@ -816,19 +816,19 @@
         <v>1</v>
       </c>
       <c r="F31" s="1">
-        <f>C31*255</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G31" s="1">
-        <f>D31*255</f>
+        <f t="shared" si="1"/>
         <v>255</v>
       </c>
       <c r="H31" s="1">
-        <f>E31*255</f>
+        <f t="shared" si="2"/>
         <v>255</v>
       </c>
       <c r="I31" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="J31" s="1" t="s">
@@ -846,19 +846,19 @@
         <v>0.745</v>
       </c>
       <c r="F32" s="5">
-        <f>C32*255</f>
+        <f t="shared" si="0"/>
         <v>189.97499999999999</v>
       </c>
       <c r="G32" s="5">
-        <f>D32*255</f>
+        <f t="shared" si="1"/>
         <v>189.97499999999999</v>
       </c>
       <c r="H32" s="5">
-        <f>E32*255</f>
+        <f t="shared" si="2"/>
         <v>189.97499999999999</v>
       </c>
       <c r="I32" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="J32" s="1" t="s">
@@ -876,19 +876,19 @@
         <v>0.41199999999999998</v>
       </c>
       <c r="F33" s="5">
-        <f>C33*255</f>
+        <f t="shared" si="0"/>
         <v>105.05999999999999</v>
       </c>
       <c r="G33" s="5">
-        <f>D33*255</f>
+        <f t="shared" si="1"/>
         <v>105.05999999999999</v>
       </c>
       <c r="H33" s="5">
-        <f>E33*255</f>
+        <f t="shared" si="2"/>
         <v>105.05999999999999</v>
       </c>
       <c r="I33" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="J33" s="1">
@@ -906,19 +906,19 @@
         <v>0.36099999999999999</v>
       </c>
       <c r="F34" s="5">
-        <f>C34*255</f>
+        <f t="shared" si="0"/>
         <v>205.02</v>
       </c>
       <c r="G34" s="5">
-        <f>D34*255</f>
+        <f t="shared" si="1"/>
         <v>92.054999999999993</v>
       </c>
       <c r="H34" s="5">
-        <f>E34*255</f>
+        <f t="shared" si="2"/>
         <v>92.054999999999993</v>
       </c>
       <c r="I34" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="J34" s="1" t="s">
@@ -936,19 +936,19 @@
         <v>0.54900000000000004</v>
       </c>
       <c r="F35" s="5">
-        <f>C35*255</f>
+        <f t="shared" si="0"/>
         <v>210.11999999999998</v>
       </c>
       <c r="G35" s="5">
-        <f>D35*255</f>
+        <f t="shared" si="1"/>
         <v>180.03</v>
       </c>
       <c r="H35" s="5">
-        <f>E35*255</f>
+        <f t="shared" si="2"/>
         <v>139.995</v>
       </c>
       <c r="I35" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="J35" s="1" t="s">

</xml_diff>